<commit_message>
bugfix v1.3 removed unnecessary code pieces
</commit_message>
<xml_diff>
--- a/tests_preprod/SBMS_AUTOTEST_RESULTS.xlsx
+++ b/tests_preprod/SBMS_AUTOTEST_RESULTS.xlsx
@@ -428,10 +428,10 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>40338526</v>
+        <v>40104986</v>
       </c>
       <c r="C1" t="n">
-        <v>40238526</v>
+        <v>40004986</v>
       </c>
       <c r="D1" t="inlineStr">
         <is>
@@ -440,7 +440,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>2024-10-20 20:49:44</t>
+          <t>2024-10-23 21:15:27</t>
         </is>
       </c>
     </row>

</xml_diff>